<commit_message>
Cambio de link a local
</commit_message>
<xml_diff>
--- a/data/roles_areas.xlsx
+++ b/data/roles_areas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Inventario\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4092164A-DB6D-4569-A4BF-5FE7820ADE38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0559817-808F-40BA-AFDF-8381C596D143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8F2D9A4D-AB14-4069-820F-8029A79ED844}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Nombre</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Area</t>
   </si>
   <si>
-    <t>Miguel</t>
-  </si>
-  <si>
     <t>Almacen</t>
   </si>
   <si>
@@ -60,6 +57,15 @@
   </si>
   <si>
     <t>Validar conteos</t>
+  </si>
+  <si>
+    <t>Piso Productivo</t>
+  </si>
+  <si>
+    <t>Miguel Carranza</t>
+  </si>
+  <si>
+    <t>Selena Lopez</t>
   </si>
 </sst>
 </file>
@@ -431,13 +437,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE56F94-5C7B-4804-99D1-BF13AFA71C59}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -450,21 +459,35 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
         <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambio de excel y codigo app.py
</commit_message>
<xml_diff>
--- a/data/roles_areas.xlsx
+++ b/data/roles_areas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Inventario\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0559817-808F-40BA-AFDF-8381C596D143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85781A1-9694-4214-B4CA-9AFABCEF166E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8F2D9A4D-AB14-4069-820F-8029A79ED844}"/>
+    <workbookView xWindow="225" yWindow="330" windowWidth="21600" windowHeight="11295" xr2:uid="{8F2D9A4D-AB14-4069-820F-8029A79ED844}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>Area</t>
   </si>
   <si>
-    <t>Almacen</t>
-  </si>
-  <si>
     <t>Soporte</t>
   </si>
   <si>
@@ -59,23 +56,32 @@
     <t>Validar conteos</t>
   </si>
   <si>
-    <t>Piso Productivo</t>
-  </si>
-  <si>
     <t>Miguel Carranza</t>
   </si>
   <si>
     <t>Selena Lopez</t>
+  </si>
+  <si>
+    <t>Warehouse</t>
+  </si>
+  <si>
+    <t>Fastenal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -101,8 +107,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,7 +447,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,35 +466,35 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambio en documento excel
</commit_message>
<xml_diff>
--- a/data/roles_areas.xlsx
+++ b/data/roles_areas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Inventario\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85781A1-9694-4214-B4CA-9AFABCEF166E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F809EF-83DD-41D2-8F22-275FA5C50434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="330" windowWidth="21600" windowHeight="11295" xr2:uid="{8F2D9A4D-AB14-4069-820F-8029A79ED844}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8F2D9A4D-AB14-4069-820F-8029A79ED844}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,36 +36,129 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>Nombre</t>
   </si>
   <si>
-    <t>Rol</t>
-  </si>
-  <si>
-    <t>Area</t>
-  </si>
-  <si>
-    <t>Soporte</t>
-  </si>
-  <si>
-    <t>Actividades</t>
-  </si>
-  <si>
-    <t>Validar conteos</t>
-  </si>
-  <si>
-    <t>Miguel Carranza</t>
-  </si>
-  <si>
-    <t>Selena Lopez</t>
-  </si>
-  <si>
-    <t>Warehouse</t>
-  </si>
-  <si>
-    <t>Fastenal</t>
+    <t>Número</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>categoria</t>
+  </si>
+  <si>
+    <t>ABREGO MORIN, CESAR EDUARDO</t>
+  </si>
+  <si>
+    <t>Counting</t>
+  </si>
+  <si>
+    <t>HOURLY DIRECT</t>
+  </si>
+  <si>
+    <t>ABUNDIS GUAJARDO, REBECA</t>
+  </si>
+  <si>
+    <t>Inventory Audit</t>
+  </si>
+  <si>
+    <t>HOURLY INDIRECT</t>
+  </si>
+  <si>
+    <t>Confidencialidad</t>
+  </si>
+  <si>
+    <t>Puesto</t>
+  </si>
+  <si>
+    <t>Cód Centro Costo</t>
+  </si>
+  <si>
+    <t>Departamento</t>
+  </si>
+  <si>
+    <t>Supervisor</t>
+  </si>
+  <si>
+    <t>Oracle Location</t>
+  </si>
+  <si>
+    <t>Shift</t>
+  </si>
+  <si>
+    <t>Responsabilidad Oracle</t>
+  </si>
+  <si>
+    <t>Comentarios / Vacaciones</t>
+  </si>
+  <si>
+    <t>DIRECTO</t>
+  </si>
+  <si>
+    <t>OPERADOR DE ENSAMBLE</t>
+  </si>
+  <si>
+    <t>Manufacturing Fabrication -Fab</t>
+  </si>
+  <si>
+    <t>JESUS SERVANDO MUNGUIA MONTELO</t>
+  </si>
+  <si>
+    <t>DH L2</t>
+  </si>
+  <si>
+    <t>MONDP</t>
+  </si>
+  <si>
+    <t>INSPECTOR DE CALIDAD</t>
+  </si>
+  <si>
+    <t>Mfg OH -Quality / Continuous I</t>
+  </si>
+  <si>
+    <t>JUAN EDGAR GUADALUPE GARCIA RU</t>
+  </si>
+  <si>
+    <t>SKID</t>
+  </si>
+  <si>
+    <t>MONSKID</t>
+  </si>
+  <si>
+    <t>ABUNDIS VILLASANA, OMAR</t>
+  </si>
+  <si>
+    <t>FRANCISCO  ALEJANDRO MONTOYA C</t>
+  </si>
+  <si>
+    <t>ABURTO BANDALA, VICTOR MANUEL</t>
+  </si>
+  <si>
+    <t>SALARY EXEMPT</t>
+  </si>
+  <si>
+    <t>SALARY</t>
+  </si>
+  <si>
+    <t>OPS PM PROJECT MANAGER</t>
+  </si>
+  <si>
+    <t>Global Operations</t>
+  </si>
+  <si>
+    <t>KURC MARIAN</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>MONMC</t>
+  </si>
+  <si>
+    <t>Location</t>
   </si>
 </sst>
 </file>
@@ -444,57 +537,224 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE56F94-5C7B-4804-99D1-BF13AFA71C59}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>20687</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>5001</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>19976</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3">
+        <v>5226</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>21142</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>5001</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>21955</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5">
+        <v>6640</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel columna SVG Id
</commit_message>
<xml_diff>
--- a/data/roles_areas.xlsx
+++ b/data/roles_areas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Inventario\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F62A857-162F-4CFC-953B-63254353417A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FF816A-4173-4516-A44D-5BDCDCFAF349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8F2D9A4D-AB14-4069-820F-8029A79ED844}"/>
   </bookViews>
@@ -5331,7 +5331,7 @@
   <dimension ref="A1:F1537"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Cambio SVG_ID, era una columna con formulas lo cambie a texto plano
</commit_message>
<xml_diff>
--- a/data/roles_areas.xlsx
+++ b/data/roles_areas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Inventario\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83EEAA2-05EA-48F6-A0D3-6B6AF4082797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F58EBE-1CCE-4B81-BFCA-60B703E8BD68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8F2D9A4D-AB14-4069-820F-8029A79ED844}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13727" uniqueCount="1616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13864" uniqueCount="1617">
   <si>
     <t>Nombre</t>
   </si>
@@ -4886,6 +4886,9 @@
   </si>
   <si>
     <t>SVG_ID</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -5346,7 +5349,7 @@
   <dimension ref="A1:F1537"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5595,8 +5598,8 @@
       <c r="E12" t="s">
         <v>31</v>
       </c>
-      <c r="F12">
-        <v>0</v>
+      <c r="F12" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -5675,8 +5678,8 @@
       <c r="E16" t="s">
         <v>33</v>
       </c>
-      <c r="F16">
-        <v>0</v>
+      <c r="F16" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -5935,8 +5938,8 @@
       <c r="E29" t="s">
         <v>33</v>
       </c>
-      <c r="F29">
-        <v>0</v>
+      <c r="F29" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -6155,8 +6158,8 @@
       <c r="E40" t="s">
         <v>33</v>
       </c>
-      <c r="F40">
-        <v>0</v>
+      <c r="F40" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -6295,8 +6298,8 @@
       <c r="E47" t="s">
         <v>33</v>
       </c>
-      <c r="F47">
-        <v>0</v>
+      <c r="F47" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -6415,8 +6418,8 @@
       <c r="E53" t="s">
         <v>31</v>
       </c>
-      <c r="F53">
-        <v>0</v>
+      <c r="F53" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -6555,8 +6558,8 @@
       <c r="E60" t="s">
         <v>33</v>
       </c>
-      <c r="F60">
-        <v>0</v>
+      <c r="F60" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -6835,8 +6838,8 @@
       <c r="E74" t="s">
         <v>33</v>
       </c>
-      <c r="F74">
-        <v>0</v>
+      <c r="F74" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -7335,8 +7338,8 @@
       <c r="E99" t="s">
         <v>31</v>
       </c>
-      <c r="F99">
-        <v>0</v>
+      <c r="F99" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -7355,8 +7358,8 @@
       <c r="E100" t="s">
         <v>33</v>
       </c>
-      <c r="F100">
-        <v>0</v>
+      <c r="F100" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -7432,8 +7435,8 @@
       <c r="D104" t="s">
         <v>50</v>
       </c>
-      <c r="F104">
-        <v>0</v>
+      <c r="F104" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -7872,8 +7875,8 @@
       <c r="E126" t="s">
         <v>33</v>
       </c>
-      <c r="F126">
-        <v>0</v>
+      <c r="F126" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -8249,8 +8252,8 @@
       <c r="D145" t="s">
         <v>50</v>
       </c>
-      <c r="F145">
-        <v>0</v>
+      <c r="F145" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
@@ -8329,8 +8332,8 @@
       <c r="E149" t="s">
         <v>31</v>
       </c>
-      <c r="F149">
-        <v>0</v>
+      <c r="F149" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
@@ -8969,8 +8972,8 @@
       <c r="E181" t="s">
         <v>33</v>
       </c>
-      <c r="F181">
-        <v>0</v>
+      <c r="F181" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
@@ -9249,8 +9252,8 @@
       <c r="E195" t="s">
         <v>33</v>
       </c>
-      <c r="F195">
-        <v>0</v>
+      <c r="F195" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
@@ -9369,8 +9372,8 @@
       <c r="E201" t="s">
         <v>33</v>
       </c>
-      <c r="F201">
-        <v>0</v>
+      <c r="F201" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
@@ -10149,8 +10152,8 @@
       <c r="E240" t="s">
         <v>53</v>
       </c>
-      <c r="F240">
-        <v>0</v>
+      <c r="F240" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
@@ -10769,8 +10772,8 @@
       <c r="E271" t="s">
         <v>31</v>
       </c>
-      <c r="F271">
-        <v>0</v>
+      <c r="F271" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
@@ -11089,8 +11092,8 @@
       <c r="E287" t="s">
         <v>31</v>
       </c>
-      <c r="F287">
-        <v>0</v>
+      <c r="F287" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.25">
@@ -11109,8 +11112,8 @@
       <c r="E288" t="s">
         <v>33</v>
       </c>
-      <c r="F288">
-        <v>0</v>
+      <c r="F288" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.25">
@@ -11249,8 +11252,8 @@
       <c r="E295" t="s">
         <v>31</v>
       </c>
-      <c r="F295">
-        <v>0</v>
+      <c r="F295" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.25">
@@ -11269,8 +11272,8 @@
       <c r="E296" t="s">
         <v>31</v>
       </c>
-      <c r="F296">
-        <v>0</v>
+      <c r="F296" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="297" spans="1:6" x14ac:dyDescent="0.25">
@@ -11489,8 +11492,8 @@
       <c r="E307" t="s">
         <v>33</v>
       </c>
-      <c r="F307">
-        <v>0</v>
+      <c r="F307" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="308" spans="1:6" x14ac:dyDescent="0.25">
@@ -11529,8 +11532,8 @@
       <c r="E309" t="s">
         <v>31</v>
       </c>
-      <c r="F309">
-        <v>0</v>
+      <c r="F309" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="310" spans="1:6" x14ac:dyDescent="0.25">
@@ -11689,8 +11692,8 @@
       <c r="E317" t="s">
         <v>33</v>
       </c>
-      <c r="F317">
-        <v>0</v>
+      <c r="F317" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="318" spans="1:6" x14ac:dyDescent="0.25">
@@ -11806,8 +11809,8 @@
       <c r="D323" t="s">
         <v>54</v>
       </c>
-      <c r="F323">
-        <v>0</v>
+      <c r="F323" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="324" spans="1:6" x14ac:dyDescent="0.25">
@@ -11866,8 +11869,8 @@
       <c r="E326" t="s">
         <v>31</v>
       </c>
-      <c r="F326">
-        <v>0</v>
+      <c r="F326" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="327" spans="1:6" x14ac:dyDescent="0.25">
@@ -11886,8 +11889,8 @@
       <c r="E327" t="s">
         <v>31</v>
       </c>
-      <c r="F327">
-        <v>0</v>
+      <c r="F327" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.25">
@@ -12146,8 +12149,8 @@
       <c r="E340" t="s">
         <v>33</v>
       </c>
-      <c r="F340">
-        <v>0</v>
+      <c r="F340" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="341" spans="1:6" x14ac:dyDescent="0.25">
@@ -12246,8 +12249,8 @@
       <c r="E345" t="s">
         <v>33</v>
       </c>
-      <c r="F345">
-        <v>0</v>
+      <c r="F345" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="346" spans="1:6" x14ac:dyDescent="0.25">
@@ -12446,8 +12449,8 @@
       <c r="E355" t="s">
         <v>31</v>
       </c>
-      <c r="F355">
-        <v>0</v>
+      <c r="F355" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="356" spans="1:6" x14ac:dyDescent="0.25">
@@ -12506,8 +12509,8 @@
       <c r="E358" t="s">
         <v>33</v>
       </c>
-      <c r="F358">
-        <v>0</v>
+      <c r="F358" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="359" spans="1:6" x14ac:dyDescent="0.25">
@@ -12523,8 +12526,8 @@
       <c r="D359" t="s">
         <v>58</v>
       </c>
-      <c r="F359">
-        <v>0</v>
+      <c r="F359" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="360" spans="1:6" x14ac:dyDescent="0.25">
@@ -12803,8 +12806,8 @@
       <c r="E373" t="s">
         <v>33</v>
       </c>
-      <c r="F373">
-        <v>0</v>
+      <c r="F373" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="374" spans="1:6" x14ac:dyDescent="0.25">
@@ -13103,8 +13106,8 @@
       <c r="E388" t="s">
         <v>33</v>
       </c>
-      <c r="F388">
-        <v>0</v>
+      <c r="F388" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="389" spans="1:6" x14ac:dyDescent="0.25">
@@ -13520,8 +13523,8 @@
       <c r="D409" t="s">
         <v>59</v>
       </c>
-      <c r="F409">
-        <v>0</v>
+      <c r="F409" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="410" spans="1:6" x14ac:dyDescent="0.25">
@@ -13540,8 +13543,8 @@
       <c r="E410" t="s">
         <v>33</v>
       </c>
-      <c r="F410">
-        <v>0</v>
+      <c r="F410" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="411" spans="1:6" x14ac:dyDescent="0.25">
@@ -13620,8 +13623,8 @@
       <c r="E414" t="s">
         <v>33</v>
       </c>
-      <c r="F414">
-        <v>0</v>
+      <c r="F414" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="415" spans="1:6" x14ac:dyDescent="0.25">
@@ -13760,8 +13763,8 @@
       <c r="E421" t="s">
         <v>33</v>
       </c>
-      <c r="F421">
-        <v>0</v>
+      <c r="F421" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="422" spans="1:6" x14ac:dyDescent="0.25">
@@ -13797,8 +13800,8 @@
       <c r="D423" t="s">
         <v>59</v>
       </c>
-      <c r="F423">
-        <v>0</v>
+      <c r="F423" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="424" spans="1:6" x14ac:dyDescent="0.25">
@@ -13857,8 +13860,8 @@
       <c r="E426" t="s">
         <v>31</v>
       </c>
-      <c r="F426">
-        <v>0</v>
+      <c r="F426" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="427" spans="1:6" x14ac:dyDescent="0.25">
@@ -14234,8 +14237,8 @@
       <c r="D445" t="s">
         <v>59</v>
       </c>
-      <c r="F445">
-        <v>0</v>
+      <c r="F445" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="446" spans="1:6" x14ac:dyDescent="0.25">
@@ -14454,8 +14457,8 @@
       <c r="E456" t="s">
         <v>31</v>
       </c>
-      <c r="F456">
-        <v>0</v>
+      <c r="F456" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="457" spans="1:6" x14ac:dyDescent="0.25">
@@ -14651,8 +14654,8 @@
       <c r="D466" t="s">
         <v>54</v>
       </c>
-      <c r="F466">
-        <v>0</v>
+      <c r="F466" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="467" spans="1:6" x14ac:dyDescent="0.25">
@@ -14908,8 +14911,8 @@
       <c r="D479" t="s">
         <v>50</v>
       </c>
-      <c r="F479">
-        <v>0</v>
+      <c r="F479" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="480" spans="1:6" x14ac:dyDescent="0.25">
@@ -15125,8 +15128,8 @@
       <c r="E490" t="s">
         <v>31</v>
       </c>
-      <c r="F490">
-        <v>0</v>
+      <c r="F490" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="491" spans="1:6" x14ac:dyDescent="0.25">
@@ -15305,8 +15308,8 @@
       <c r="E499" t="s">
         <v>33</v>
       </c>
-      <c r="F499">
-        <v>0</v>
+      <c r="F499" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="500" spans="1:6" x14ac:dyDescent="0.25">
@@ -15325,8 +15328,8 @@
       <c r="E500" t="s">
         <v>33</v>
       </c>
-      <c r="F500">
-        <v>0</v>
+      <c r="F500" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="501" spans="1:6" x14ac:dyDescent="0.25">
@@ -16122,8 +16125,8 @@
       <c r="E540" t="s">
         <v>33</v>
       </c>
-      <c r="F540">
-        <v>0</v>
+      <c r="F540" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="541" spans="1:6" x14ac:dyDescent="0.25">
@@ -16502,8 +16505,8 @@
       <c r="E559" t="s">
         <v>33</v>
       </c>
-      <c r="F559">
-        <v>0</v>
+      <c r="F559" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="560" spans="1:6" x14ac:dyDescent="0.25">
@@ -16522,8 +16525,8 @@
       <c r="E560" t="s">
         <v>33</v>
       </c>
-      <c r="F560">
-        <v>0</v>
+      <c r="F560" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="561" spans="1:6" x14ac:dyDescent="0.25">
@@ -17562,8 +17565,8 @@
       <c r="E612" t="s">
         <v>33</v>
       </c>
-      <c r="F612">
-        <v>0</v>
+      <c r="F612" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="613" spans="1:6" x14ac:dyDescent="0.25">
@@ -18022,8 +18025,8 @@
       <c r="E635" t="s">
         <v>33</v>
       </c>
-      <c r="F635">
-        <v>0</v>
+      <c r="F635" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="636" spans="1:6" x14ac:dyDescent="0.25">
@@ -18522,8 +18525,8 @@
       <c r="E660" t="s">
         <v>33</v>
       </c>
-      <c r="F660">
-        <v>0</v>
+      <c r="F660" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="661" spans="1:6" x14ac:dyDescent="0.25">
@@ -18542,8 +18545,8 @@
       <c r="E661" t="s">
         <v>33</v>
       </c>
-      <c r="F661">
-        <v>0</v>
+      <c r="F661" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="662" spans="1:6" x14ac:dyDescent="0.25">
@@ -18582,8 +18585,8 @@
       <c r="E663" t="s">
         <v>33</v>
       </c>
-      <c r="F663">
-        <v>0</v>
+      <c r="F663" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="664" spans="1:6" x14ac:dyDescent="0.25">
@@ -18702,8 +18705,8 @@
       <c r="E669" t="s">
         <v>33</v>
       </c>
-      <c r="F669">
-        <v>0</v>
+      <c r="F669" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="670" spans="1:6" x14ac:dyDescent="0.25">
@@ -18742,8 +18745,8 @@
       <c r="E671" t="s">
         <v>33</v>
       </c>
-      <c r="F671">
-        <v>0</v>
+      <c r="F671" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="672" spans="1:6" x14ac:dyDescent="0.25">
@@ -18962,8 +18965,8 @@
       <c r="E682" t="s">
         <v>33</v>
       </c>
-      <c r="F682">
-        <v>0</v>
+      <c r="F682" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="683" spans="1:6" x14ac:dyDescent="0.25">
@@ -19082,8 +19085,8 @@
       <c r="E688" t="s">
         <v>33</v>
       </c>
-      <c r="F688">
-        <v>0</v>
+      <c r="F688" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="689" spans="1:6" x14ac:dyDescent="0.25">
@@ -19402,8 +19405,8 @@
       <c r="E704" t="s">
         <v>33</v>
       </c>
-      <c r="F704">
-        <v>0</v>
+      <c r="F704" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="705" spans="1:6" x14ac:dyDescent="0.25">
@@ -19459,8 +19462,8 @@
       <c r="D707" t="s">
         <v>61</v>
       </c>
-      <c r="F707">
-        <v>0</v>
+      <c r="F707" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="708" spans="1:6" x14ac:dyDescent="0.25">
@@ -19499,8 +19502,8 @@
       <c r="E709" t="s">
         <v>33</v>
       </c>
-      <c r="F709">
-        <v>0</v>
+      <c r="F709" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="710" spans="1:6" x14ac:dyDescent="0.25">
@@ -19599,8 +19602,8 @@
       <c r="E714" t="s">
         <v>31</v>
       </c>
-      <c r="F714">
-        <v>0</v>
+      <c r="F714" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="715" spans="1:6" x14ac:dyDescent="0.25">
@@ -20136,8 +20139,8 @@
       <c r="D741" t="s">
         <v>61</v>
       </c>
-      <c r="F741">
-        <v>0</v>
+      <c r="F741" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="742" spans="1:6" x14ac:dyDescent="0.25">
@@ -20196,8 +20199,8 @@
       <c r="E744" t="s">
         <v>31</v>
       </c>
-      <c r="F744">
-        <v>0</v>
+      <c r="F744" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="745" spans="1:6" x14ac:dyDescent="0.25">
@@ -20376,8 +20379,8 @@
       <c r="E753" t="s">
         <v>33</v>
       </c>
-      <c r="F753">
-        <v>0</v>
+      <c r="F753" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="754" spans="1:6" x14ac:dyDescent="0.25">
@@ -20456,8 +20459,8 @@
       <c r="E757" t="s">
         <v>33</v>
       </c>
-      <c r="F757">
-        <v>0</v>
+      <c r="F757" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="758" spans="1:6" x14ac:dyDescent="0.25">
@@ -20596,8 +20599,8 @@
       <c r="E764" t="s">
         <v>31</v>
       </c>
-      <c r="F764">
-        <v>0</v>
+      <c r="F764" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="765" spans="1:6" x14ac:dyDescent="0.25">
@@ -20736,8 +20739,8 @@
       <c r="E771" t="s">
         <v>31</v>
       </c>
-      <c r="F771">
-        <v>0</v>
+      <c r="F771" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="772" spans="1:6" x14ac:dyDescent="0.25">
@@ -20773,8 +20776,8 @@
       <c r="D773" t="s">
         <v>50</v>
       </c>
-      <c r="F773">
-        <v>0</v>
+      <c r="F773" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="774" spans="1:6" x14ac:dyDescent="0.25">
@@ -21233,8 +21236,8 @@
       <c r="E796" t="s">
         <v>33</v>
       </c>
-      <c r="F796">
-        <v>0</v>
+      <c r="F796" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="797" spans="1:6" x14ac:dyDescent="0.25">
@@ -21253,8 +21256,8 @@
       <c r="E797" t="s">
         <v>31</v>
       </c>
-      <c r="F797">
-        <v>0</v>
+      <c r="F797" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="798" spans="1:6" x14ac:dyDescent="0.25">
@@ -21353,8 +21356,8 @@
       <c r="E802" t="s">
         <v>31</v>
       </c>
-      <c r="F802">
-        <v>0</v>
+      <c r="F802" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="803" spans="1:6" x14ac:dyDescent="0.25">
@@ -21593,8 +21596,8 @@
       <c r="E814" t="s">
         <v>33</v>
       </c>
-      <c r="F814">
-        <v>0</v>
+      <c r="F814" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="815" spans="1:6" x14ac:dyDescent="0.25">
@@ -22193,8 +22196,8 @@
       <c r="E844" t="s">
         <v>31</v>
       </c>
-      <c r="F844">
-        <v>0</v>
+      <c r="F844" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="845" spans="1:6" x14ac:dyDescent="0.25">
@@ -22313,8 +22316,8 @@
       <c r="E850" t="s">
         <v>33</v>
       </c>
-      <c r="F850">
-        <v>0</v>
+      <c r="F850" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="851" spans="1:6" x14ac:dyDescent="0.25">
@@ -22473,8 +22476,8 @@
       <c r="E858" t="s">
         <v>31</v>
       </c>
-      <c r="F858">
-        <v>0</v>
+      <c r="F858" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="859" spans="1:6" x14ac:dyDescent="0.25">
@@ -22553,8 +22556,8 @@
       <c r="E862" t="s">
         <v>31</v>
       </c>
-      <c r="F862">
-        <v>0</v>
+      <c r="F862" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="863" spans="1:6" x14ac:dyDescent="0.25">
@@ -22670,8 +22673,8 @@
       <c r="D868" t="s">
         <v>50</v>
       </c>
-      <c r="F868">
-        <v>0</v>
+      <c r="F868" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="869" spans="1:6" x14ac:dyDescent="0.25">
@@ -23090,8 +23093,8 @@
       <c r="E889" t="s">
         <v>33</v>
       </c>
-      <c r="F889">
-        <v>0</v>
+      <c r="F889" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="890" spans="1:6" x14ac:dyDescent="0.25">
@@ -23490,8 +23493,8 @@
       <c r="E909" t="s">
         <v>33</v>
       </c>
-      <c r="F909">
-        <v>0</v>
+      <c r="F909" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="910" spans="1:6" x14ac:dyDescent="0.25">
@@ -23647,8 +23650,8 @@
       <c r="D917" t="s">
         <v>61</v>
       </c>
-      <c r="F917">
-        <v>0</v>
+      <c r="F917" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="918" spans="1:6" x14ac:dyDescent="0.25">
@@ -24527,8 +24530,8 @@
       <c r="E961" t="s">
         <v>31</v>
       </c>
-      <c r="F961">
-        <v>0</v>
+      <c r="F961" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="962" spans="1:6" x14ac:dyDescent="0.25">
@@ -24847,8 +24850,8 @@
       <c r="E977" t="s">
         <v>33</v>
       </c>
-      <c r="F977">
-        <v>0</v>
+      <c r="F977" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="978" spans="1:6" x14ac:dyDescent="0.25">
@@ -24904,8 +24907,8 @@
       <c r="D980" t="s">
         <v>50</v>
       </c>
-      <c r="F980">
-        <v>0</v>
+      <c r="F980" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="981" spans="1:6" x14ac:dyDescent="0.25">
@@ -25724,8 +25727,8 @@
       <c r="E1021" t="s">
         <v>33</v>
       </c>
-      <c r="F1021">
-        <v>0</v>
+      <c r="F1021" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1022" spans="1:6" x14ac:dyDescent="0.25">
@@ -25864,8 +25867,8 @@
       <c r="E1028" t="s">
         <v>33</v>
       </c>
-      <c r="F1028">
-        <v>0</v>
+      <c r="F1028" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1029" spans="1:6" x14ac:dyDescent="0.25">
@@ -25921,8 +25924,8 @@
       <c r="D1031" t="s">
         <v>50</v>
       </c>
-      <c r="F1031">
-        <v>0</v>
+      <c r="F1031" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1032" spans="1:6" x14ac:dyDescent="0.25">
@@ -26201,8 +26204,8 @@
       <c r="E1045" t="s">
         <v>31</v>
       </c>
-      <c r="F1045">
-        <v>0</v>
+      <c r="F1045" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1046" spans="1:6" x14ac:dyDescent="0.25">
@@ -26341,8 +26344,8 @@
       <c r="E1052" t="s">
         <v>33</v>
       </c>
-      <c r="F1052">
-        <v>0</v>
+      <c r="F1052" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1053" spans="1:6" x14ac:dyDescent="0.25">
@@ -26521,8 +26524,8 @@
       <c r="E1061" t="s">
         <v>33</v>
       </c>
-      <c r="F1061">
-        <v>0</v>
+      <c r="F1061" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1062" spans="1:6" x14ac:dyDescent="0.25">
@@ -26841,8 +26844,8 @@
       <c r="E1077" t="s">
         <v>33</v>
       </c>
-      <c r="F1077">
-        <v>0</v>
+      <c r="F1077" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1078" spans="1:6" x14ac:dyDescent="0.25">
@@ -27221,8 +27224,8 @@
       <c r="E1096" t="s">
         <v>31</v>
       </c>
-      <c r="F1096">
-        <v>0</v>
+      <c r="F1096" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1097" spans="1:6" x14ac:dyDescent="0.25">
@@ -27541,8 +27544,8 @@
       <c r="E1112" t="s">
         <v>31</v>
       </c>
-      <c r="F1112">
-        <v>0</v>
+      <c r="F1112" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1113" spans="1:6" x14ac:dyDescent="0.25">
@@ -27841,8 +27844,8 @@
       <c r="E1127" t="s">
         <v>31</v>
       </c>
-      <c r="F1127">
-        <v>0</v>
+      <c r="F1127" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1128" spans="1:6" x14ac:dyDescent="0.25">
@@ -28041,8 +28044,8 @@
       <c r="E1137" t="s">
         <v>33</v>
       </c>
-      <c r="F1137">
-        <v>0</v>
+      <c r="F1137" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1138" spans="1:6" x14ac:dyDescent="0.25">
@@ -28061,8 +28064,8 @@
       <c r="E1138" t="s">
         <v>31</v>
       </c>
-      <c r="F1138">
-        <v>0</v>
+      <c r="F1138" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1139" spans="1:6" x14ac:dyDescent="0.25">
@@ -28141,8 +28144,8 @@
       <c r="E1142" t="s">
         <v>31</v>
       </c>
-      <c r="F1142">
-        <v>0</v>
+      <c r="F1142" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1143" spans="1:6" x14ac:dyDescent="0.25">
@@ -28441,8 +28444,8 @@
       <c r="E1157" t="s">
         <v>33</v>
       </c>
-      <c r="F1157">
-        <v>0</v>
+      <c r="F1157" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1158" spans="1:6" x14ac:dyDescent="0.25">
@@ -28458,8 +28461,8 @@
       <c r="D1158" t="s">
         <v>62</v>
       </c>
-      <c r="F1158">
-        <v>0</v>
+      <c r="F1158" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1159" spans="1:6" x14ac:dyDescent="0.25">
@@ -28518,8 +28521,8 @@
       <c r="E1161" t="s">
         <v>33</v>
       </c>
-      <c r="F1161">
-        <v>0</v>
+      <c r="F1161" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1162" spans="1:6" x14ac:dyDescent="0.25">
@@ -28758,8 +28761,8 @@
       <c r="E1173" t="s">
         <v>33</v>
       </c>
-      <c r="F1173">
-        <v>0</v>
+      <c r="F1173" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1174" spans="1:6" x14ac:dyDescent="0.25">
@@ -29238,8 +29241,8 @@
       <c r="E1197" t="s">
         <v>31</v>
       </c>
-      <c r="F1197">
-        <v>0</v>
+      <c r="F1197" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1198" spans="1:6" x14ac:dyDescent="0.25">
@@ -29255,8 +29258,8 @@
       <c r="D1198" t="s">
         <v>50</v>
       </c>
-      <c r="F1198">
-        <v>0</v>
+      <c r="F1198" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1199" spans="1:6" x14ac:dyDescent="0.25">
@@ -29295,8 +29298,8 @@
       <c r="E1200" t="s">
         <v>33</v>
       </c>
-      <c r="F1200">
-        <v>0</v>
+      <c r="F1200" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1201" spans="1:6" x14ac:dyDescent="0.25">
@@ -29552,8 +29555,8 @@
       <c r="D1213" t="s">
         <v>50</v>
       </c>
-      <c r="F1213">
-        <v>0</v>
+      <c r="F1213" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1214" spans="1:6" x14ac:dyDescent="0.25">
@@ -30092,8 +30095,8 @@
       <c r="E1240" t="s">
         <v>33</v>
       </c>
-      <c r="F1240">
-        <v>0</v>
+      <c r="F1240" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1241" spans="1:6" x14ac:dyDescent="0.25">
@@ -30712,8 +30715,8 @@
       <c r="E1271" t="s">
         <v>31</v>
       </c>
-      <c r="F1271">
-        <v>0</v>
+      <c r="F1271" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1272" spans="1:6" x14ac:dyDescent="0.25">
@@ -31352,8 +31355,8 @@
       <c r="E1303" t="s">
         <v>31</v>
       </c>
-      <c r="F1303">
-        <v>0</v>
+      <c r="F1303" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1304" spans="1:6" x14ac:dyDescent="0.25">
@@ -31392,8 +31395,8 @@
       <c r="E1305" t="s">
         <v>33</v>
       </c>
-      <c r="F1305">
-        <v>0</v>
+      <c r="F1305" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1306" spans="1:6" x14ac:dyDescent="0.25">
@@ -31492,8 +31495,8 @@
       <c r="E1310" t="s">
         <v>31</v>
       </c>
-      <c r="F1310">
-        <v>0</v>
+      <c r="F1310" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1311" spans="1:6" x14ac:dyDescent="0.25">
@@ -31672,8 +31675,8 @@
       <c r="E1319" t="s">
         <v>33</v>
       </c>
-      <c r="F1319">
-        <v>0</v>
+      <c r="F1319" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1320" spans="1:6" x14ac:dyDescent="0.25">
@@ -31792,8 +31795,8 @@
       <c r="E1325" t="s">
         <v>31</v>
       </c>
-      <c r="F1325">
-        <v>0</v>
+      <c r="F1325" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1326" spans="1:6" x14ac:dyDescent="0.25">
@@ -31872,8 +31875,8 @@
       <c r="E1329" t="s">
         <v>31</v>
       </c>
-      <c r="F1329">
-        <v>0</v>
+      <c r="F1329" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1330" spans="1:6" x14ac:dyDescent="0.25">
@@ -32052,8 +32055,8 @@
       <c r="E1338" t="s">
         <v>31</v>
       </c>
-      <c r="F1338">
-        <v>0</v>
+      <c r="F1338" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1339" spans="1:6" x14ac:dyDescent="0.25">
@@ -32212,8 +32215,8 @@
       <c r="E1346" t="s">
         <v>31</v>
       </c>
-      <c r="F1346">
-        <v>0</v>
+      <c r="F1346" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1347" spans="1:6" x14ac:dyDescent="0.25">
@@ -32532,8 +32535,8 @@
       <c r="E1362" t="s">
         <v>31</v>
       </c>
-      <c r="F1362">
-        <v>0</v>
+      <c r="F1362" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1363" spans="1:6" x14ac:dyDescent="0.25">
@@ -33412,8 +33415,8 @@
       <c r="E1406" t="s">
         <v>33</v>
       </c>
-      <c r="F1406">
-        <v>0</v>
+      <c r="F1406" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1407" spans="1:6" x14ac:dyDescent="0.25">
@@ -33449,8 +33452,8 @@
       <c r="D1408" t="s">
         <v>50</v>
       </c>
-      <c r="F1408">
-        <v>0</v>
+      <c r="F1408" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1409" spans="1:6" x14ac:dyDescent="0.25">
@@ -33589,8 +33592,8 @@
       <c r="E1415" t="s">
         <v>31</v>
       </c>
-      <c r="F1415">
-        <v>0</v>
+      <c r="F1415" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1416" spans="1:6" x14ac:dyDescent="0.25">
@@ -33666,8 +33669,8 @@
       <c r="D1419" t="s">
         <v>50</v>
       </c>
-      <c r="F1419">
-        <v>0</v>
+      <c r="F1419" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1420" spans="1:6" x14ac:dyDescent="0.25">
@@ -33943,8 +33946,8 @@
       <c r="D1433" t="s">
         <v>50</v>
       </c>
-      <c r="F1433">
-        <v>0</v>
+      <c r="F1433" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1434" spans="1:6" x14ac:dyDescent="0.25">
@@ -33963,8 +33966,8 @@
       <c r="E1434" t="s">
         <v>33</v>
       </c>
-      <c r="F1434">
-        <v>0</v>
+      <c r="F1434" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1435" spans="1:6" x14ac:dyDescent="0.25">
@@ -34083,8 +34086,8 @@
       <c r="E1440" t="s">
         <v>31</v>
       </c>
-      <c r="F1440">
-        <v>0</v>
+      <c r="F1440" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1441" spans="1:6" x14ac:dyDescent="0.25">
@@ -34143,8 +34146,8 @@
       <c r="E1443" t="s">
         <v>31</v>
       </c>
-      <c r="F1443">
-        <v>0</v>
+      <c r="F1443" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1444" spans="1:6" x14ac:dyDescent="0.25">
@@ -34360,8 +34363,8 @@
       <c r="D1454" t="s">
         <v>61</v>
       </c>
-      <c r="F1454">
-        <v>0</v>
+      <c r="F1454" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1455" spans="1:6" x14ac:dyDescent="0.25">
@@ -34480,8 +34483,8 @@
       <c r="E1460" t="s">
         <v>31</v>
       </c>
-      <c r="F1460">
-        <v>0</v>
+      <c r="F1460" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1461" spans="1:6" x14ac:dyDescent="0.25">
@@ -34540,8 +34543,8 @@
       <c r="E1463" t="s">
         <v>31</v>
       </c>
-      <c r="F1463">
-        <v>0</v>
+      <c r="F1463" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1464" spans="1:6" x14ac:dyDescent="0.25">
@@ -34600,8 +34603,8 @@
       <c r="E1466" t="s">
         <v>33</v>
       </c>
-      <c r="F1466">
-        <v>0</v>
+      <c r="F1466" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1467" spans="1:6" x14ac:dyDescent="0.25">
@@ -34620,8 +34623,8 @@
       <c r="E1467" t="s">
         <v>33</v>
       </c>
-      <c r="F1467">
-        <v>0</v>
+      <c r="F1467" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1468" spans="1:6" x14ac:dyDescent="0.25">
@@ -34680,8 +34683,8 @@
       <c r="E1470" t="s">
         <v>33</v>
       </c>
-      <c r="F1470">
-        <v>0</v>
+      <c r="F1470" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1471" spans="1:6" x14ac:dyDescent="0.25">
@@ -34780,8 +34783,8 @@
       <c r="E1475" t="s">
         <v>31</v>
       </c>
-      <c r="F1475">
-        <v>0</v>
+      <c r="F1475" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1476" spans="1:6" x14ac:dyDescent="0.25">
@@ -35040,8 +35043,8 @@
       <c r="E1488" t="s">
         <v>31</v>
       </c>
-      <c r="F1488">
-        <v>0</v>
+      <c r="F1488" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1489" spans="1:6" x14ac:dyDescent="0.25">
@@ -35300,8 +35303,8 @@
       <c r="E1501" t="s">
         <v>33</v>
       </c>
-      <c r="F1501">
-        <v>0</v>
+      <c r="F1501" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1502" spans="1:6" x14ac:dyDescent="0.25">
@@ -35580,8 +35583,8 @@
       <c r="E1515" t="s">
         <v>31</v>
       </c>
-      <c r="F1515">
-        <v>0</v>
+      <c r="F1515" t="s">
+        <v>1616</v>
       </c>
     </row>
     <row r="1516" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>